<commit_message>
ENH: addl calcs, rerun all, and update draft for resubmission
</commit_message>
<xml_diff>
--- a/sup_table_2.xlsx
+++ b/sup_table_2.xlsx
@@ -505,7 +505,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0.035</t>
+          <t>0.003</t>
         </is>
       </c>
     </row>
@@ -555,7 +555,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>0.020</t>
+          <t>0.011</t>
         </is>
       </c>
     </row>
@@ -605,7 +605,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>0.025</t>
+          <t>0.008</t>
         </is>
       </c>
     </row>
@@ -801,7 +801,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.019</t>
+          <t>0.005</t>
         </is>
       </c>
     </row>
@@ -851,7 +851,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.028</t>
+          <t>0.018</t>
         </is>
       </c>
     </row>
@@ -901,7 +901,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.076</t>
+          <t>0.013</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>0.132</t>
+          <t>0.133</t>
         </is>
       </c>
     </row>
@@ -1097,7 +1097,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.023</t>
+          <t>0.006</t>
         </is>
       </c>
     </row>
@@ -1147,7 +1147,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.034</t>
+          <t>0.021</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.119</t>
+          <t>0.017</t>
         </is>
       </c>
     </row>
@@ -1393,7 +1393,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>0.072</t>
+          <t>0.008</t>
         </is>
       </c>
     </row>
@@ -1443,7 +1443,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>0.055</t>
+          <t>0.026</t>
         </is>
       </c>
     </row>
@@ -1493,7 +1493,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>0.060</t>
+          <t>0.018</t>
         </is>
       </c>
     </row>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>0.050</t>
+          <t>0.009</t>
         </is>
       </c>
     </row>
@@ -1739,7 +1739,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>0.047</t>
+          <t>0.027</t>
         </is>
       </c>
     </row>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>0.085</t>
+          <t>0.023</t>
         </is>
       </c>
     </row>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>0.028</t>
+          <t>0.010</t>
         </is>
       </c>
     </row>
@@ -2035,7 +2035,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>0.060</t>
+          <t>0.033</t>
         </is>
       </c>
     </row>
@@ -2085,7 +2085,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>0.142</t>
+          <t>0.026</t>
         </is>
       </c>
     </row>
@@ -2281,7 +2281,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>0.066</t>
+          <t>0.010</t>
         </is>
       </c>
     </row>
@@ -2331,7 +2331,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>0.070</t>
+          <t>0.036</t>
         </is>
       </c>
     </row>
@@ -2381,7 +2381,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>0.122</t>
+          <t>0.029</t>
         </is>
       </c>
     </row>
@@ -2481,7 +2481,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>0.250</t>
+          <t>0.253</t>
         </is>
       </c>
     </row>
@@ -2577,7 +2577,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>0.079</t>
+          <t>0.013</t>
         </is>
       </c>
     </row>
@@ -2627,7 +2627,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>0.068</t>
+          <t>0.044</t>
         </is>
       </c>
     </row>
@@ -2677,7 +2677,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>0.231</t>
+          <t>0.033</t>
         </is>
       </c>
     </row>
@@ -2777,7 +2777,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>0.275</t>
+          <t>0.274</t>
         </is>
       </c>
     </row>
@@ -2873,7 +2873,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>0.039</t>
+          <t>0.014</t>
         </is>
       </c>
     </row>
@@ -2923,7 +2923,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>0.085</t>
+          <t>0.044</t>
         </is>
       </c>
     </row>
@@ -2973,7 +2973,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>0.102</t>
+          <t>0.040</t>
         </is>
       </c>
     </row>
@@ -3073,7 +3073,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>0.298</t>
+          <t>0.295</t>
         </is>
       </c>
     </row>
@@ -3169,7 +3169,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>0.082</t>
+          <t>0.013</t>
         </is>
       </c>
     </row>
@@ -3219,7 +3219,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>0.079</t>
+          <t>0.050</t>
         </is>
       </c>
     </row>
@@ -3269,7 +3269,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>0.164</t>
+          <t>0.040</t>
         </is>
       </c>
     </row>
@@ -3465,7 +3465,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>0.132</t>
+          <t>0.018</t>
         </is>
       </c>
     </row>
@@ -3515,7 +3515,7 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>0.097</t>
+          <t>0.060</t>
         </is>
       </c>
     </row>
@@ -3565,7 +3565,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>0.124</t>
+          <t>0.049</t>
         </is>
       </c>
     </row>
@@ -3665,7 +3665,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>0.362</t>
+          <t>0.363</t>
         </is>
       </c>
     </row>
@@ -3761,7 +3761,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>0.105</t>
+          <t>0.022</t>
         </is>
       </c>
     </row>
@@ -3811,7 +3811,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>0.125</t>
+          <t>0.064</t>
         </is>
       </c>
     </row>
@@ -3861,7 +3861,7 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>0.245</t>
+          <t>0.051</t>
         </is>
       </c>
     </row>
@@ -3961,7 +3961,7 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>0.411</t>
+          <t>0.397</t>
         </is>
       </c>
     </row>
@@ -4057,7 +4057,7 @@
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>0.121</t>
+          <t>0.019</t>
         </is>
       </c>
     </row>
@@ -4107,7 +4107,7 @@
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>0.104</t>
+          <t>0.065</t>
         </is>
       </c>
     </row>
@@ -4157,7 +4157,7 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>0.470</t>
+          <t>0.053</t>
         </is>
       </c>
     </row>
@@ -4257,7 +4257,7 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>0.448</t>
+          <t>0.454</t>
         </is>
       </c>
     </row>
@@ -4353,7 +4353,7 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>0.066</t>
+          <t>0.023</t>
         </is>
       </c>
     </row>
@@ -4403,7 +4403,7 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>0.132</t>
+          <t>0.073</t>
         </is>
       </c>
     </row>
@@ -4453,7 +4453,7 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>0.183</t>
+          <t>0.054</t>
         </is>
       </c>
     </row>
@@ -4553,7 +4553,7 @@
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>0.503</t>
+          <t>0.523</t>
         </is>
       </c>
     </row>
@@ -4649,7 +4649,7 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>0.075</t>
+          <t>0.025</t>
         </is>
       </c>
     </row>
@@ -4699,7 +4699,7 @@
       </c>
       <c r="J88" t="inlineStr">
         <is>
-          <t>0.129</t>
+          <t>0.091</t>
         </is>
       </c>
     </row>
@@ -4749,7 +4749,7 @@
       </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>0.278</t>
+          <t>0.065</t>
         </is>
       </c>
     </row>
@@ -4799,7 +4799,7 @@
       </c>
       <c r="J90" t="inlineStr">
         <is>
-          <t>0.257</t>
+          <t>0.258</t>
         </is>
       </c>
     </row>
@@ -4849,7 +4849,7 @@
       </c>
       <c r="J91" t="inlineStr">
         <is>
-          <t>0.551</t>
+          <t>0.578</t>
         </is>
       </c>
     </row>
@@ -4945,7 +4945,7 @@
       </c>
       <c r="J93" t="inlineStr">
         <is>
-          <t>0.104</t>
+          <t>0.031</t>
         </is>
       </c>
     </row>
@@ -4995,7 +4995,7 @@
       </c>
       <c r="J94" t="inlineStr">
         <is>
-          <t>0.154</t>
+          <t>0.098</t>
         </is>
       </c>
     </row>
@@ -5045,7 +5045,7 @@
       </c>
       <c r="J95" t="inlineStr">
         <is>
-          <t>0.267</t>
+          <t>0.065</t>
         </is>
       </c>
     </row>
@@ -5095,7 +5095,7 @@
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>0.294</t>
+          <t>0.293</t>
         </is>
       </c>
     </row>
@@ -5145,7 +5145,7 @@
       </c>
       <c r="J97" t="inlineStr">
         <is>
-          <t>0.703</t>
+          <t>0.623</t>
         </is>
       </c>
     </row>
@@ -5241,7 +5241,7 @@
       </c>
       <c r="J99" t="inlineStr">
         <is>
-          <t>0.095</t>
+          <t>0.033</t>
         </is>
       </c>
     </row>
@@ -5291,7 +5291,7 @@
       </c>
       <c r="J100" t="inlineStr">
         <is>
-          <t>0.208</t>
+          <t>0.115</t>
         </is>
       </c>
     </row>
@@ -5341,7 +5341,7 @@
       </c>
       <c r="J101" t="inlineStr">
         <is>
-          <t>0.234</t>
+          <t>0.087</t>
         </is>
       </c>
     </row>
@@ -5391,7 +5391,7 @@
       </c>
       <c r="J102" t="inlineStr">
         <is>
-          <t>0.341</t>
+          <t>0.339</t>
         </is>
       </c>
     </row>
@@ -5441,7 +5441,7 @@
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t>0.842</t>
+          <t>0.812</t>
         </is>
       </c>
     </row>
@@ -5537,7 +5537,7 @@
       </c>
       <c r="J105" t="inlineStr">
         <is>
-          <t>0.125</t>
+          <t>0.042</t>
         </is>
       </c>
     </row>
@@ -5587,7 +5587,7 @@
       </c>
       <c r="J106" t="inlineStr">
         <is>
-          <t>0.211</t>
+          <t>0.137</t>
         </is>
       </c>
     </row>
@@ -5637,7 +5637,7 @@
       </c>
       <c r="J107" t="inlineStr">
         <is>
-          <t>0.511</t>
+          <t>0.120</t>
         </is>
       </c>
     </row>
@@ -5737,7 +5737,7 @@
       </c>
       <c r="J109" t="inlineStr">
         <is>
-          <t>0.937</t>
+          <t>0.970</t>
         </is>
       </c>
     </row>
@@ -5833,7 +5833,7 @@
       </c>
       <c r="J111" t="inlineStr">
         <is>
-          <t>0.429</t>
+          <t>0.063</t>
         </is>
       </c>
     </row>
@@ -5883,7 +5883,7 @@
       </c>
       <c r="J112" t="inlineStr">
         <is>
-          <t>0.314</t>
+          <t>0.215</t>
         </is>
       </c>
     </row>
@@ -5933,7 +5933,7 @@
       </c>
       <c r="J113" t="inlineStr">
         <is>
-          <t>0.944</t>
+          <t>0.193</t>
         </is>
       </c>
     </row>
@@ -5983,7 +5983,7 @@
       </c>
       <c r="J114" t="inlineStr">
         <is>
-          <t>0.612</t>
+          <t>0.611</t>
         </is>
       </c>
     </row>
@@ -6033,7 +6033,7 @@
       </c>
       <c r="J115" t="inlineStr">
         <is>
-          <t>1.333</t>
+          <t>1.307</t>
         </is>
       </c>
     </row>

</xml_diff>